<commit_message>
feat : Stage 3,4 추가
</commit_message>
<xml_diff>
--- a/기획/PIE_레벨디자인_엑셀시트.xlsx
+++ b/기획/PIE_레벨디자인_엑셀시트.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\기획수업 기말 게임제작\PIE_Project_B_Midterm\기획\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\기획수업 기말 게임제작\PIE_Project_B_1214_2\기획\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA46DA2-80F0-47B1-9D05-F59DB347CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2953189-9C2C-44EC-AD4C-FED767CC4654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1425" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>

</xml_diff>